<commit_message>
new skills, key words *
add new skills, fix key words, add * before keyword
</commit_message>
<xml_diff>
--- a/FinalProject/Codebase/datasource/ds_kw.xlsx
+++ b/FinalProject/Codebase/datasource/ds_kw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelapaiva/Documents/GitHub/DataScience/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26169DC2-509C-4646-8F59-5C3DFE534BCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE9F6B5-DCF7-0445-A4DA-E6D7D036E08E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="87">
   <si>
     <t>kwID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>SQL</t>
-  </si>
-  <si>
     <t>BigData</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>Predictive Modeling</t>
-  </si>
-  <si>
     <t>Physics</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>PhD's</t>
   </si>
   <si>
-    <t>data Scientist</t>
-  </si>
-  <si>
     <t>MBA</t>
   </si>
   <si>
@@ -241,16 +232,55 @@
     <t xml:space="preserve"> ML </t>
   </si>
   <si>
-    <t xml:space="preserve">R </t>
-  </si>
-  <si>
-    <t>R,</t>
-  </si>
-  <si>
     <t>R)</t>
   </si>
   <si>
     <t>,R,</t>
+  </si>
+  <si>
+    <t>*SQL</t>
+  </si>
+  <si>
+    <t>*R,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*R </t>
+  </si>
+  <si>
+    <t>*R.</t>
+  </si>
+  <si>
+    <t>Identify clusters in data</t>
+  </si>
+  <si>
+    <t>Identify clusters</t>
+  </si>
+  <si>
+    <t>clusters in data</t>
+  </si>
+  <si>
+    <t>Predict future outcomes</t>
+  </si>
+  <si>
+    <t>statistical analysis</t>
+  </si>
+  <si>
+    <t>Deep Learning</t>
+  </si>
+  <si>
+    <t>Pandas</t>
+  </si>
+  <si>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Kafta</t>
+  </si>
+  <si>
+    <t>Predictive Model</t>
+  </si>
+  <si>
+    <t>no-SQL</t>
   </si>
 </sst>
 </file>
@@ -640,15 +670,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -686,8 +716,8 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -701,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -715,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -729,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -743,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
@@ -771,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
@@ -785,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -799,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>5</v>
@@ -813,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
@@ -827,7 +857,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
@@ -840,8 +870,8 @@
       <c r="B14" s="2">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>74</v>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
@@ -855,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
@@ -869,7 +899,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>5</v>
@@ -883,7 +913,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>5</v>
@@ -894,10 +924,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>5</v>
@@ -908,10 +938,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>5</v>
@@ -925,7 +955,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>5</v>
@@ -939,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
@@ -950,10 +980,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>5</v>
@@ -964,10 +994,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>5</v>
@@ -978,10 +1008,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>5</v>
@@ -995,7 +1025,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>5</v>
@@ -1009,7 +1039,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>5</v>
@@ -1023,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
@@ -1034,10 +1064,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>5</v>
@@ -1048,10 +1078,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>5</v>
@@ -1062,10 +1092,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -1076,10 +1106,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
@@ -1090,10 +1120,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -1104,10 +1134,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
@@ -1121,7 +1151,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -1135,7 +1165,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1146,10 +1176,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1160,10 +1190,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -1177,7 +1207,7 @@
         <v>24</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>
@@ -1191,7 +1221,7 @@
         <v>24</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>5</v>
@@ -1202,10 +1232,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
@@ -1216,10 +1246,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>5</v>
@@ -1230,10 +1260,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>5</v>
@@ -1244,10 +1274,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>5</v>
@@ -1258,10 +1288,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>5</v>
@@ -1272,10 +1302,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>5</v>
@@ -1286,10 +1316,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>5</v>
@@ -1300,15 +1330,14 @@
         <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -1318,21 +1347,22 @@
         <v>32</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>5</v>
@@ -1346,7 +1376,7 @@
         <v>33</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>5</v>
@@ -1360,7 +1390,7 @@
         <v>33</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>5</v>
@@ -1374,7 +1404,7 @@
         <v>33</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>5</v>
@@ -1385,10 +1415,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>5</v>
@@ -1399,10 +1429,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>5</v>
@@ -1413,10 +1443,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>5</v>
@@ -1427,10 +1457,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>5</v>
@@ -1441,10 +1471,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>5</v>
@@ -1455,10 +1485,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>5</v>
@@ -1469,10 +1499,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>5</v>
@@ -1483,10 +1513,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>5</v>
@@ -1497,10 +1527,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>5</v>
@@ -1511,10 +1541,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>5</v>
@@ -1525,10 +1555,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>5</v>
@@ -1539,10 +1569,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>5</v>
@@ -1553,10 +1583,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>5</v>
@@ -1567,10 +1597,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>5</v>
@@ -1581,25 +1611,24 @@
         <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>5</v>
@@ -1611,10 +1640,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>5</v>
@@ -1626,10 +1655,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>5</v>
@@ -1641,10 +1670,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>5</v>
@@ -1656,10 +1685,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>5</v>
@@ -1671,13 +1700,168 @@
         <v>72</v>
       </c>
       <c r="B73" s="2">
+        <v>52</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2">
+        <v>53</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
         <v>54</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>69</v>
+      <c r="C75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2">
+        <v>54</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2">
+        <v>54</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2">
+        <v>35</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2">
+        <v>8</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2">
+        <v>9</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2">
+        <v>55</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2">
+        <v>56</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2">
+        <v>57</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2">
+        <v>47</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>